<commit_message>
Data Driven Testing Approach is added for ContactsPage using DataProvider in TestNG and reading data from excel using POI library Still 1st row is ignored and other rows are read and added from the excelfile, other rows from excel are read and values of fields is entered fine Some other minor changes are also made
</commit_message>
<xml_diff>
--- a/src/main/java/com/cogmento/ui/data/TestData.xlsx
+++ b/src/main/java/com/cogmento/ui/data/TestData.xlsx
@@ -1,23 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{43374462-207B-44C7-B93F-AA2FB63C2C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2688" yWindow="3288" windowWidth="14880" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Mr Aziz</t>
+  </si>
+  <si>
+    <t>Mr Farhan</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>mfa@yopmail.com</t>
+  </si>
+  <si>
+    <t>Babar</t>
+  </si>
+  <si>
+    <t>Mr Siraj</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>shq@yopmail.com</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +74,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -43,17 +114,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -100,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,9 +216,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,6 +268,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -343,36 +460,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{8A9E375A-53D9-4C8F-B206-24941AB7F3EE}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{79F1FBDB-166B-4A2C-BDFC-33DADEA1BE99}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>